<commit_message>
OCA Actualizada al 19/11/21
</commit_message>
<xml_diff>
--- a/Gastos.xlsx
+++ b/Gastos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
   <si>
     <t>Julio</t>
   </si>
@@ -204,6 +204,18 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Legacy (Remeras Trabajo)</t>
+  </si>
+  <si>
+    <t>Filtro de Agua</t>
+  </si>
+  <si>
+    <t>Legacy (Jean para salir)</t>
+  </si>
+  <si>
+    <t>Recarga celular</t>
   </si>
 </sst>
 </file>
@@ -706,11 +718,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="6" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,7 +1548,7 @@
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -1580,7 +1592,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -1624,7 +1636,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1652,7 +1664,7 @@
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -1672,7 +1684,7 @@
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>54</v>
       </c>
@@ -1692,7 +1704,7 @@
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>55</v>
       </c>
@@ -1712,7 +1724,7 @@
       <c r="M38" s="7"/>
       <c r="N38" s="7"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>56</v>
       </c>
@@ -1732,7 +1744,7 @@
       <c r="M39" s="7"/>
       <c r="N39" s="7"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -1752,10 +1764,15 @@
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
+      <c r="D41" s="7">
+        <v>1935</v>
+      </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -1767,26 +1784,61 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>60</v>
+      </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D42" s="7">
+        <v>329</v>
+      </c>
+      <c r="E42" s="7">
+        <v>329</v>
+      </c>
+      <c r="F42" s="7">
+        <v>329</v>
+      </c>
+      <c r="G42" s="7">
+        <v>329</v>
+      </c>
+      <c r="H42" s="7">
+        <v>329</v>
+      </c>
+      <c r="I42" s="7">
+        <v>329</v>
+      </c>
+      <c r="J42" s="7">
+        <v>329</v>
+      </c>
+      <c r="K42" s="7">
+        <v>329</v>
+      </c>
+      <c r="L42" s="7">
+        <v>329</v>
+      </c>
+      <c r="M42" s="7">
+        <v>329</v>
+      </c>
+      <c r="N42" s="7">
+        <v>329</v>
+      </c>
+      <c r="O42" s="7">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>61</v>
+      </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
+      <c r="D43" s="7">
+        <v>1345</v>
+      </c>
+      <c r="E43" s="7">
+        <v>1345</v>
+      </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
@@ -1797,10 +1849,15 @@
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>62</v>
+      </c>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
+      <c r="D44" s="7">
+        <v>100</v>
+      </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
@@ -1812,7 +1869,7 @@
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -1827,7 +1884,7 @@
       <c r="M45" s="7"/>
       <c r="N45" s="7"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -1842,7 +1899,7 @@
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -1857,7 +1914,7 @@
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -1892,56 +1949,56 @@
         <v>13</v>
       </c>
       <c r="B50" s="2">
-        <f>SUM(B8:B49)</f>
+        <f t="shared" ref="B50:N50" si="0">SUM(B8:B49)</f>
         <v>13190</v>
       </c>
       <c r="C50" s="2">
-        <f>SUM(C8:C49)</f>
+        <f t="shared" si="0"/>
         <v>16881</v>
       </c>
       <c r="D50" s="2">
-        <f>SUM(D8:D49)</f>
-        <v>10481</v>
+        <f t="shared" si="0"/>
+        <v>14190</v>
       </c>
       <c r="E50" s="2">
-        <f>SUM(E8:E49)</f>
-        <v>6596</v>
+        <f t="shared" si="0"/>
+        <v>8270</v>
       </c>
       <c r="F50" s="2">
-        <f>SUM(F8:F49)</f>
-        <v>5323</v>
+        <f t="shared" si="0"/>
+        <v>5652</v>
       </c>
       <c r="G50" s="2">
-        <f>SUM(G8:G49)</f>
-        <v>5323</v>
+        <f t="shared" si="0"/>
+        <v>5652</v>
       </c>
       <c r="H50" s="2">
-        <f>SUM(H8:H49)</f>
-        <v>5203</v>
+        <f t="shared" si="0"/>
+        <v>5532</v>
       </c>
       <c r="I50" s="2">
-        <f>SUM(I8:I49)</f>
-        <v>3651</v>
+        <f t="shared" si="0"/>
+        <v>3980</v>
       </c>
       <c r="J50" s="2">
-        <f>SUM(J8:J49)</f>
-        <v>3651</v>
+        <f t="shared" si="0"/>
+        <v>3980</v>
       </c>
       <c r="K50" s="2">
-        <f>SUM(K8:K49)</f>
-        <v>3651</v>
+        <f t="shared" si="0"/>
+        <v>3980</v>
       </c>
       <c r="L50" s="2">
-        <f>SUM(L8:L49)</f>
-        <v>3651</v>
+        <f t="shared" si="0"/>
+        <v>3980</v>
       </c>
       <c r="M50" s="2">
-        <f>SUM(M8:M49)</f>
-        <v>3651</v>
+        <f t="shared" si="0"/>
+        <v>3980</v>
       </c>
       <c r="N50" s="2">
-        <f>SUM(N8:N49)</f>
-        <v>3651</v>
+        <f t="shared" si="0"/>
+        <v>3980</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -2084,7 +2141,7 @@
         <v>3500</v>
       </c>
       <c r="D55">
-        <v>2500</v>
+        <v>2200</v>
       </c>
       <c r="E55">
         <v>2500</v>
@@ -2122,55 +2179,55 @@
         <v>21</v>
       </c>
       <c r="B56" s="2">
-        <f t="shared" ref="B56:N56" si="0">SUM(B52:B55)</f>
+        <f t="shared" ref="B56:N56" si="1">SUM(B52:B55)</f>
         <v>8250</v>
       </c>
       <c r="C56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7750</v>
       </c>
       <c r="D56" s="2">
-        <f t="shared" si="0"/>
-        <v>9150</v>
+        <f t="shared" si="1"/>
+        <v>8850</v>
       </c>
       <c r="E56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6750</v>
       </c>
       <c r="F56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7956</v>
       </c>
       <c r="G56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6750</v>
       </c>
       <c r="H56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7956</v>
       </c>
       <c r="I56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6750</v>
       </c>
       <c r="J56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7956</v>
       </c>
       <c r="K56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6750</v>
       </c>
       <c r="L56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7956</v>
       </c>
       <c r="M56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6750</v>
       </c>
       <c r="N56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7956</v>
       </c>
     </row>
@@ -2241,56 +2298,56 @@
         <v>22</v>
       </c>
       <c r="B61" s="6">
-        <f t="shared" ref="B61:N61" si="1">SUM(B50+B56+B58)</f>
+        <f t="shared" ref="B61:N61" si="2">SUM(B50+B56+B58)</f>
         <v>31440</v>
       </c>
       <c r="C61" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34631</v>
       </c>
       <c r="D61" s="6">
-        <f t="shared" si="1"/>
-        <v>29631</v>
+        <f t="shared" si="2"/>
+        <v>33040</v>
       </c>
       <c r="E61" s="6">
-        <f t="shared" si="1"/>
-        <v>23346</v>
+        <f t="shared" si="2"/>
+        <v>25020</v>
       </c>
       <c r="F61" s="6">
-        <f t="shared" si="1"/>
-        <v>23279</v>
+        <f t="shared" si="2"/>
+        <v>23608</v>
       </c>
       <c r="G61" s="6">
-        <f t="shared" si="1"/>
-        <v>22073</v>
+        <f t="shared" si="2"/>
+        <v>22402</v>
       </c>
       <c r="H61" s="6">
-        <f t="shared" si="1"/>
-        <v>23159</v>
+        <f t="shared" si="2"/>
+        <v>23488</v>
       </c>
       <c r="I61" s="6">
-        <f t="shared" si="1"/>
-        <v>20401</v>
+        <f t="shared" si="2"/>
+        <v>20730</v>
       </c>
       <c r="J61" s="6">
-        <f t="shared" si="1"/>
-        <v>21607</v>
+        <f t="shared" si="2"/>
+        <v>21936</v>
       </c>
       <c r="K61" s="6">
-        <f t="shared" si="1"/>
-        <v>20401</v>
+        <f t="shared" si="2"/>
+        <v>20730</v>
       </c>
       <c r="L61" s="6">
-        <f t="shared" si="1"/>
-        <v>21607</v>
+        <f t="shared" si="2"/>
+        <v>21936</v>
       </c>
       <c r="M61" s="6">
-        <f t="shared" si="1"/>
-        <v>20401</v>
+        <f t="shared" si="2"/>
+        <v>20730</v>
       </c>
       <c r="N61" s="6">
-        <f t="shared" si="1"/>
-        <v>21607</v>
+        <f t="shared" si="2"/>
+        <v>21936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OCA Actualizada al 21/01/22
</commit_message>
<xml_diff>
--- a/Gastos.xlsx
+++ b/Gastos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
   <si>
     <t>Julio</t>
   </si>
@@ -273,6 +273,12 @@
   </si>
   <si>
     <t>Recarga celular (actualizado al 19/01/21)</t>
+  </si>
+  <si>
+    <t>Libro</t>
+  </si>
+  <si>
+    <t>Bicicleta Spinning</t>
   </si>
 </sst>
 </file>
@@ -719,11 +725,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L78"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <pane ySplit="6" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1637,20 +1643,46 @@
       <c r="K41" s="7"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>83</v>
+      </c>
       <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
+      <c r="C42" s="7">
+        <v>1080</v>
+      </c>
+      <c r="D42" s="7">
+        <v>1080</v>
+      </c>
+      <c r="E42" s="7">
+        <v>1080</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1080</v>
+      </c>
+      <c r="G42" s="7">
+        <v>1080</v>
+      </c>
+      <c r="H42" s="7">
+        <v>1080</v>
+      </c>
+      <c r="I42" s="7">
+        <v>1080</v>
+      </c>
+      <c r="J42" s="7">
+        <v>1080</v>
+      </c>
+      <c r="K42" s="7">
+        <v>1080</v>
+      </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>82</v>
+      </c>
       <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
+      <c r="C43" s="7">
+        <v>450</v>
+      </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
@@ -1661,995 +1693,1019 @@
       <c r="K43" s="7"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="18">
-        <f>SUM(B8:B43)</f>
+      <c r="B46" s="18">
+        <f t="shared" ref="B46:K46" si="0">SUM(B8:B45)</f>
         <v>13527</v>
       </c>
-      <c r="C44" s="18">
-        <f>SUM(C8:C43)</f>
-        <v>9000</v>
-      </c>
-      <c r="D44" s="18">
-        <f>SUM(D8:D43)</f>
-        <v>7150</v>
-      </c>
-      <c r="E44" s="18">
-        <f>SUM(E8:E43)</f>
-        <v>7030</v>
-      </c>
-      <c r="F44" s="18">
-        <f>SUM(F8:F43)</f>
-        <v>6107</v>
-      </c>
-      <c r="G44" s="18">
-        <f>SUM(G8:G43)</f>
-        <v>5750</v>
-      </c>
-      <c r="H44" s="18">
-        <f>SUM(H8:H43)</f>
-        <v>5750</v>
-      </c>
-      <c r="I44" s="18">
-        <f>SUM(I8:I43)</f>
-        <v>5750</v>
-      </c>
-      <c r="J44" s="18">
-        <f>SUM(J8:J43)</f>
-        <v>5750</v>
-      </c>
-      <c r="K44" s="18">
-        <f>SUM(K8:K43)</f>
-        <v>5750</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="C46" s="18">
+        <f t="shared" si="0"/>
+        <v>10530</v>
+      </c>
+      <c r="D46" s="18">
+        <f t="shared" si="0"/>
+        <v>8230</v>
+      </c>
+      <c r="E46" s="18">
+        <f t="shared" si="0"/>
+        <v>8110</v>
+      </c>
+      <c r="F46" s="18">
+        <f t="shared" si="0"/>
+        <v>7187</v>
+      </c>
+      <c r="G46" s="18">
+        <f t="shared" si="0"/>
+        <v>6830</v>
+      </c>
+      <c r="H46" s="18">
+        <f t="shared" si="0"/>
+        <v>6830</v>
+      </c>
+      <c r="I46" s="18">
+        <f t="shared" si="0"/>
+        <v>6830</v>
+      </c>
+      <c r="J46" s="18">
+        <f t="shared" si="0"/>
+        <v>6830</v>
+      </c>
+      <c r="K46" s="18">
+        <f t="shared" si="0"/>
+        <v>6830</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46">
-        <v>2550</v>
-      </c>
-      <c r="C46">
-        <v>2550</v>
-      </c>
-      <c r="D46">
-        <v>2550</v>
-      </c>
-      <c r="E46">
-        <v>2550</v>
-      </c>
-      <c r="F46">
-        <v>2550</v>
-      </c>
-      <c r="G46">
-        <v>2550</v>
-      </c>
-      <c r="H46">
-        <v>2550</v>
-      </c>
-      <c r="I46">
-        <v>2550</v>
-      </c>
-      <c r="J46">
-        <v>2550</v>
-      </c>
-      <c r="K46">
-        <v>2550</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>13</v>
-      </c>
-      <c r="C47">
-        <v>1206</v>
-      </c>
-      <c r="E47">
-        <v>1206</v>
-      </c>
-      <c r="G47">
-        <v>1206</v>
-      </c>
-      <c r="I47">
-        <v>1206</v>
-      </c>
-      <c r="K47">
-        <v>1206</v>
-      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B48">
-        <v>1700</v>
+        <v>2550</v>
       </c>
       <c r="C48">
-        <v>1700</v>
+        <v>2550</v>
       </c>
       <c r="D48">
-        <v>1700</v>
+        <v>2550</v>
       </c>
       <c r="E48">
-        <v>1700</v>
+        <v>2550</v>
       </c>
       <c r="F48">
-        <v>1700</v>
+        <v>2550</v>
       </c>
       <c r="G48">
-        <v>1700</v>
+        <v>2550</v>
       </c>
       <c r="H48">
-        <v>1700</v>
+        <v>2550</v>
       </c>
       <c r="I48">
-        <v>1700</v>
+        <v>2550</v>
       </c>
       <c r="J48">
-        <v>1700</v>
+        <v>2550</v>
       </c>
       <c r="K48">
-        <v>1700</v>
+        <v>2550</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>15</v>
-      </c>
-      <c r="B49">
-        <v>2500</v>
+        <v>13</v>
       </c>
       <c r="C49">
-        <v>2500</v>
-      </c>
-      <c r="D49">
-        <v>2500</v>
+        <v>1206</v>
       </c>
       <c r="E49">
-        <v>2500</v>
-      </c>
-      <c r="F49">
-        <v>2500</v>
+        <v>1206</v>
       </c>
       <c r="G49">
-        <v>2500</v>
-      </c>
-      <c r="H49">
-        <v>2500</v>
+        <v>1206</v>
       </c>
       <c r="I49">
-        <v>2500</v>
-      </c>
-      <c r="J49">
-        <v>2500</v>
+        <v>1206</v>
       </c>
       <c r="K49">
-        <v>2500</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="B50">
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="C50">
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="D50">
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="E50">
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="F50">
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="G50">
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="H50">
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="I50">
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="J50">
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="K50">
-        <v>1000</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>2500</v>
+      </c>
+      <c r="C51">
+        <v>2500</v>
+      </c>
+      <c r="D51">
+        <v>2500</v>
+      </c>
+      <c r="E51">
+        <v>2500</v>
+      </c>
+      <c r="F51">
+        <v>2500</v>
+      </c>
+      <c r="G51">
+        <v>2500</v>
+      </c>
+      <c r="H51">
+        <v>2500</v>
+      </c>
+      <c r="I51">
+        <v>2500</v>
+      </c>
+      <c r="J51">
+        <v>2500</v>
+      </c>
+      <c r="K51">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52">
+        <v>1000</v>
+      </c>
+      <c r="C52">
+        <v>1000</v>
+      </c>
+      <c r="D52">
+        <v>1000</v>
+      </c>
+      <c r="E52">
+        <v>1000</v>
+      </c>
+      <c r="F52">
+        <v>1000</v>
+      </c>
+      <c r="G52">
+        <v>1000</v>
+      </c>
+      <c r="H52">
+        <v>1000</v>
+      </c>
+      <c r="I52">
+        <v>1000</v>
+      </c>
+      <c r="J52">
+        <v>1000</v>
+      </c>
+      <c r="K52">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>67</v>
       </c>
-      <c r="B51">
+      <c r="B53">
         <v>1000</v>
       </c>
-      <c r="C51">
+      <c r="C53">
         <v>1000</v>
       </c>
-      <c r="D51">
+      <c r="D53">
         <v>1000</v>
       </c>
-      <c r="E51">
+      <c r="E53">
         <v>1000</v>
       </c>
-      <c r="F51">
+      <c r="F53">
         <v>1000</v>
       </c>
-      <c r="G51">
+      <c r="G53">
         <v>1000</v>
       </c>
-      <c r="H51">
+      <c r="H53">
         <v>1000</v>
       </c>
-      <c r="I51">
+      <c r="I53">
         <v>1000</v>
       </c>
-      <c r="J51">
+      <c r="J53">
         <v>1000</v>
       </c>
-      <c r="K51">
+      <c r="K53">
         <v>1000</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="2">
-        <f t="shared" ref="B52:K52" si="0">SUM(B46:B51)</f>
+      <c r="B54" s="2">
+        <f t="shared" ref="B54:K54" si="1">SUM(B48:B53)</f>
         <v>8750</v>
       </c>
-      <c r="C52" s="2">
-        <f t="shared" si="0"/>
+      <c r="C54" s="2">
+        <f t="shared" si="1"/>
         <v>9956</v>
       </c>
-      <c r="D52" s="2">
-        <f t="shared" si="0"/>
+      <c r="D54" s="2">
+        <f t="shared" si="1"/>
         <v>8750</v>
       </c>
-      <c r="E52" s="2">
-        <f t="shared" si="0"/>
+      <c r="E54" s="2">
+        <f t="shared" si="1"/>
         <v>9956</v>
       </c>
-      <c r="F52" s="2">
-        <f t="shared" si="0"/>
+      <c r="F54" s="2">
+        <f t="shared" si="1"/>
         <v>8750</v>
       </c>
-      <c r="G52" s="2">
-        <f t="shared" si="0"/>
+      <c r="G54" s="2">
+        <f t="shared" si="1"/>
         <v>9956</v>
       </c>
-      <c r="H52" s="2">
-        <f t="shared" si="0"/>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
         <v>8750</v>
       </c>
-      <c r="I52" s="2">
-        <f t="shared" si="0"/>
+      <c r="I54" s="2">
+        <f t="shared" si="1"/>
         <v>9956</v>
       </c>
-      <c r="J52" s="2">
-        <f t="shared" si="0"/>
+      <c r="J54" s="2">
+        <f t="shared" si="1"/>
         <v>8750</v>
       </c>
-      <c r="K52" s="2">
-        <f t="shared" si="0"/>
+      <c r="K54" s="2">
+        <f t="shared" si="1"/>
         <v>9956</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54">
-        <v>600</v>
-      </c>
-      <c r="C54">
-        <v>600</v>
-      </c>
-      <c r="D54">
-        <v>600</v>
-      </c>
-      <c r="E54">
-        <v>600</v>
-      </c>
-      <c r="F54">
-        <v>600</v>
-      </c>
-      <c r="G54">
-        <v>600</v>
-      </c>
-      <c r="H54">
-        <v>600</v>
-      </c>
-      <c r="I54">
-        <v>600</v>
-      </c>
-      <c r="J54">
-        <v>600</v>
-      </c>
-      <c r="K54">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55">
-        <v>1600</v>
-      </c>
-      <c r="C55">
-        <v>1600</v>
-      </c>
-      <c r="D55">
-        <v>1600</v>
-      </c>
-      <c r="E55">
-        <v>1600</v>
-      </c>
-      <c r="F55">
-        <v>1600</v>
-      </c>
-      <c r="G55">
-        <v>1600</v>
-      </c>
-      <c r="H55">
-        <v>1600</v>
-      </c>
-      <c r="I55">
-        <v>1600</v>
-      </c>
-      <c r="J55">
-        <v>1600</v>
-      </c>
-      <c r="K55">
-        <v>1600</v>
-      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B56">
-        <v>2400</v>
+        <v>600</v>
       </c>
       <c r="C56">
-        <v>2400</v>
+        <v>600</v>
       </c>
       <c r="D56">
-        <v>2400</v>
+        <v>600</v>
       </c>
       <c r="E56">
-        <v>2400</v>
+        <v>600</v>
       </c>
       <c r="F56">
-        <v>2400</v>
+        <v>600</v>
       </c>
       <c r="G56">
-        <v>2400</v>
+        <v>600</v>
       </c>
       <c r="H56">
-        <v>2400</v>
+        <v>600</v>
       </c>
       <c r="I56">
-        <v>2400</v>
+        <v>600</v>
       </c>
       <c r="J56">
-        <v>2400</v>
+        <v>600</v>
       </c>
       <c r="K56">
-        <v>2400</v>
+        <v>600</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57">
+        <v>1600</v>
+      </c>
+      <c r="C57">
+        <v>1600</v>
+      </c>
+      <c r="D57">
+        <v>1600</v>
+      </c>
+      <c r="E57">
+        <v>1600</v>
+      </c>
+      <c r="F57">
+        <v>1600</v>
+      </c>
+      <c r="G57">
+        <v>1600</v>
+      </c>
+      <c r="H57">
+        <v>1600</v>
+      </c>
+      <c r="I57">
+        <v>1600</v>
+      </c>
+      <c r="J57">
+        <v>1600</v>
+      </c>
+      <c r="K57">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58">
+        <v>2400</v>
+      </c>
+      <c r="C58">
+        <v>2400</v>
+      </c>
+      <c r="D58">
+        <v>2400</v>
+      </c>
+      <c r="E58">
+        <v>2400</v>
+      </c>
+      <c r="F58">
+        <v>2400</v>
+      </c>
+      <c r="G58">
+        <v>2400</v>
+      </c>
+      <c r="H58">
+        <v>2400</v>
+      </c>
+      <c r="I58">
+        <v>2400</v>
+      </c>
+      <c r="J58">
+        <v>2400</v>
+      </c>
+      <c r="K58">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>64</v>
       </c>
-      <c r="B57">
+      <c r="B59">
         <v>450</v>
       </c>
-      <c r="C57">
+      <c r="C59">
         <v>450</v>
       </c>
-      <c r="D57">
+      <c r="D59">
         <v>450</v>
       </c>
-      <c r="E57">
+      <c r="E59">
         <v>450</v>
       </c>
-      <c r="F57">
+      <c r="F59">
         <v>450</v>
       </c>
-      <c r="G57">
+      <c r="G59">
         <v>450</v>
       </c>
-      <c r="H57">
+      <c r="H59">
         <v>450</v>
       </c>
-      <c r="I57">
+      <c r="I59">
         <v>450</v>
       </c>
-      <c r="J57">
+      <c r="J59">
         <v>450</v>
       </c>
-      <c r="K57">
+      <c r="K59">
         <v>450</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="2">
-        <f t="shared" ref="B58:K58" si="1">SUM(B54:B57)</f>
+      <c r="B60" s="2">
+        <f t="shared" ref="B60:K60" si="2">SUM(B56:B59)</f>
         <v>5050</v>
       </c>
-      <c r="C58" s="2">
-        <f t="shared" si="1"/>
+      <c r="C60" s="2">
+        <f t="shared" si="2"/>
         <v>5050</v>
       </c>
-      <c r="D58" s="2">
-        <f t="shared" si="1"/>
+      <c r="D60" s="2">
+        <f t="shared" si="2"/>
         <v>5050</v>
       </c>
-      <c r="E58" s="2">
-        <f t="shared" si="1"/>
+      <c r="E60" s="2">
+        <f t="shared" si="2"/>
         <v>5050</v>
       </c>
-      <c r="F58" s="2">
-        <f t="shared" si="1"/>
+      <c r="F60" s="2">
+        <f t="shared" si="2"/>
         <v>5050</v>
       </c>
-      <c r="G58" s="2">
-        <f t="shared" si="1"/>
+      <c r="G60" s="2">
+        <f t="shared" si="2"/>
         <v>5050</v>
       </c>
-      <c r="H58" s="2">
-        <f t="shared" si="1"/>
+      <c r="H60" s="2">
+        <f t="shared" si="2"/>
         <v>5050</v>
       </c>
-      <c r="I58" s="2">
-        <f t="shared" si="1"/>
+      <c r="I60" s="2">
+        <f t="shared" si="2"/>
         <v>5050</v>
       </c>
-      <c r="J58" s="2">
-        <f t="shared" si="1"/>
+      <c r="J60" s="2">
+        <f t="shared" si="2"/>
         <v>5050</v>
       </c>
-      <c r="K58" s="2">
-        <f t="shared" si="1"/>
+      <c r="K60" s="2">
+        <f t="shared" si="2"/>
         <v>5050</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60">
-        <v>500</v>
-      </c>
-      <c r="C60">
-        <v>500</v>
-      </c>
-      <c r="D60">
-        <v>500</v>
-      </c>
-      <c r="E60">
-        <v>500</v>
-      </c>
-      <c r="F60">
-        <v>500</v>
-      </c>
-      <c r="G60">
-        <v>500</v>
-      </c>
-      <c r="H60">
-        <v>500</v>
-      </c>
-      <c r="I60">
-        <v>500</v>
-      </c>
-      <c r="J60">
-        <v>500</v>
-      </c>
-      <c r="K60">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>65</v>
-      </c>
-      <c r="B61">
-        <v>300</v>
-      </c>
-      <c r="C61">
-        <v>300</v>
-      </c>
-      <c r="D61">
-        <v>300</v>
-      </c>
-      <c r="E61">
-        <v>300</v>
-      </c>
-      <c r="F61">
-        <v>300</v>
-      </c>
-      <c r="G61">
-        <v>300</v>
-      </c>
-      <c r="H61">
-        <v>300</v>
-      </c>
-      <c r="I61">
-        <v>300</v>
-      </c>
-      <c r="J61">
-        <v>300</v>
-      </c>
-      <c r="K61">
-        <v>300</v>
-      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62">
+        <v>500</v>
+      </c>
+      <c r="C62">
+        <v>500</v>
+      </c>
+      <c r="D62">
+        <v>500</v>
+      </c>
+      <c r="E62">
+        <v>500</v>
+      </c>
+      <c r="F62">
+        <v>500</v>
+      </c>
+      <c r="G62">
+        <v>500</v>
+      </c>
+      <c r="H62">
+        <v>500</v>
+      </c>
+      <c r="I62">
+        <v>500</v>
+      </c>
+      <c r="J62">
+        <v>500</v>
+      </c>
+      <c r="K62">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63">
+        <v>300</v>
+      </c>
+      <c r="C63">
+        <v>300</v>
+      </c>
+      <c r="D63">
+        <v>300</v>
+      </c>
+      <c r="E63">
+        <v>300</v>
+      </c>
+      <c r="F63">
+        <v>300</v>
+      </c>
+      <c r="G63">
+        <v>300</v>
+      </c>
+      <c r="H63">
+        <v>300</v>
+      </c>
+      <c r="I63">
+        <v>300</v>
+      </c>
+      <c r="J63">
+        <v>300</v>
+      </c>
+      <c r="K63">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>58</v>
       </c>
-      <c r="B62">
+      <c r="B64">
         <v>300</v>
       </c>
-      <c r="C62">
+      <c r="C64">
         <v>300</v>
       </c>
-      <c r="D62">
+      <c r="D64">
         <v>300</v>
       </c>
-      <c r="E62">
+      <c r="E64">
         <v>300</v>
       </c>
-      <c r="F62">
+      <c r="F64">
         <v>300</v>
       </c>
-      <c r="G62">
+      <c r="G64">
         <v>300</v>
       </c>
-      <c r="H62">
+      <c r="H64">
         <v>300</v>
       </c>
-      <c r="I62">
+      <c r="I64">
         <v>300</v>
       </c>
-      <c r="J62">
+      <c r="J64">
         <v>300</v>
       </c>
-      <c r="K62">
+      <c r="K64">
         <v>300</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="2">
-        <f t="shared" ref="B63:K63" si="2">SUM(B60:B62)</f>
+      <c r="B65" s="2">
+        <f t="shared" ref="B65:K65" si="3">SUM(B62:B64)</f>
         <v>1100</v>
       </c>
-      <c r="C63" s="2">
-        <f t="shared" si="2"/>
+      <c r="C65" s="2">
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
-      <c r="D63" s="2">
-        <f t="shared" si="2"/>
+      <c r="D65" s="2">
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
-      <c r="E63" s="2">
-        <f t="shared" si="2"/>
+      <c r="E65" s="2">
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
-      <c r="F63" s="2">
-        <f t="shared" si="2"/>
+      <c r="F65" s="2">
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
-      <c r="G63" s="2">
-        <f t="shared" si="2"/>
+      <c r="G65" s="2">
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
-      <c r="H63" s="2">
-        <f t="shared" si="2"/>
+      <c r="H65" s="2">
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
-      <c r="I63" s="2">
-        <f t="shared" si="2"/>
+      <c r="I65" s="2">
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
-      <c r="J63" s="2">
-        <f t="shared" si="2"/>
+      <c r="J65" s="2">
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
-      <c r="K63" s="2">
-        <f t="shared" si="2"/>
+      <c r="K65" s="2">
+        <f t="shared" si="3"/>
         <v>1100</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>63</v>
       </c>
-      <c r="D66">
+      <c r="D68">
         <v>6700</v>
       </c>
-      <c r="E66">
-        <v>11200</v>
-      </c>
-      <c r="F66">
-        <v>11200</v>
-      </c>
-      <c r="G66">
-        <v>11200</v>
-      </c>
-      <c r="H66">
-        <v>11200</v>
-      </c>
-      <c r="I66">
-        <v>11200</v>
-      </c>
-      <c r="J66">
-        <v>11200</v>
-      </c>
-      <c r="K66">
-        <v>11200</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="E68">
+        <v>6200</v>
+      </c>
+      <c r="F68">
+        <v>6200</v>
+      </c>
+      <c r="G68">
+        <v>6200</v>
+      </c>
+      <c r="H68">
+        <v>6200</v>
+      </c>
+      <c r="I68">
+        <v>6200</v>
+      </c>
+      <c r="J68">
+        <v>6200</v>
+      </c>
+      <c r="K68">
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B67" s="2">
-        <f t="shared" ref="B67:K67" si="3">SUM(B65:B66)</f>
+      <c r="B69" s="2">
+        <f t="shared" ref="B69:K69" si="4">SUM(B67:B68)</f>
         <v>0</v>
       </c>
-      <c r="C67" s="2">
-        <f t="shared" si="3"/>
+      <c r="C69" s="2">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D67" s="2">
-        <f t="shared" si="3"/>
+      <c r="D69" s="2">
+        <f t="shared" si="4"/>
         <v>6700</v>
       </c>
-      <c r="E67" s="2">
-        <f t="shared" si="3"/>
-        <v>11200</v>
-      </c>
-      <c r="F67" s="2">
-        <f t="shared" si="3"/>
-        <v>11200</v>
-      </c>
-      <c r="G67" s="2">
-        <f t="shared" si="3"/>
-        <v>11200</v>
-      </c>
-      <c r="H67" s="2">
-        <f t="shared" si="3"/>
-        <v>11200</v>
-      </c>
-      <c r="I67" s="2">
-        <f t="shared" si="3"/>
-        <v>11200</v>
-      </c>
-      <c r="J67" s="2">
-        <f t="shared" si="3"/>
-        <v>11200</v>
-      </c>
-      <c r="K67" s="2">
-        <f t="shared" si="3"/>
-        <v>11200</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
+      <c r="E69" s="2">
+        <f t="shared" si="4"/>
+        <v>6200</v>
+      </c>
+      <c r="F69" s="2">
+        <f t="shared" si="4"/>
+        <v>6200</v>
+      </c>
+      <c r="G69" s="2">
+        <f t="shared" si="4"/>
+        <v>6200</v>
+      </c>
+      <c r="H69" s="2">
+        <f t="shared" si="4"/>
+        <v>6200</v>
+      </c>
+      <c r="I69" s="2">
+        <f t="shared" si="4"/>
+        <v>6200</v>
+      </c>
+      <c r="J69" s="2">
+        <f t="shared" si="4"/>
+        <v>6200</v>
+      </c>
+      <c r="K69" s="2">
+        <f t="shared" si="4"/>
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="16">
-        <f t="shared" ref="B69:K69" si="4">SUM(B44,B52,B58,B63,B67)</f>
+      <c r="B71" s="16">
+        <f t="shared" ref="B71:K71" si="5">SUM(B46,B54,B60,B65,B69)</f>
         <v>28427</v>
       </c>
-      <c r="C69" s="16">
-        <f t="shared" si="4"/>
-        <v>25106</v>
-      </c>
-      <c r="D69" s="16">
-        <f t="shared" si="4"/>
-        <v>28750</v>
-      </c>
-      <c r="E69" s="16">
-        <f t="shared" si="4"/>
-        <v>34336</v>
-      </c>
-      <c r="F69" s="16">
-        <f t="shared" si="4"/>
-        <v>32207</v>
-      </c>
-      <c r="G69" s="16">
-        <f t="shared" si="4"/>
-        <v>33056</v>
-      </c>
-      <c r="H69" s="16">
-        <f t="shared" si="4"/>
-        <v>31850</v>
-      </c>
-      <c r="I69" s="16">
-        <f t="shared" si="4"/>
-        <v>33056</v>
-      </c>
-      <c r="J69" s="16">
-        <f t="shared" si="4"/>
-        <v>31850</v>
-      </c>
-      <c r="K69" s="16">
-        <f t="shared" si="4"/>
-        <v>33056</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="C71" s="16">
+        <f t="shared" si="5"/>
+        <v>26636</v>
+      </c>
+      <c r="D71" s="16">
+        <f t="shared" si="5"/>
+        <v>29830</v>
+      </c>
+      <c r="E71" s="16">
+        <f t="shared" si="5"/>
+        <v>30416</v>
+      </c>
+      <c r="F71" s="16">
+        <f t="shared" si="5"/>
+        <v>28287</v>
+      </c>
+      <c r="G71" s="16">
+        <f t="shared" si="5"/>
+        <v>29136</v>
+      </c>
+      <c r="H71" s="16">
+        <f t="shared" si="5"/>
+        <v>27930</v>
+      </c>
+      <c r="I71" s="16">
+        <f t="shared" si="5"/>
+        <v>29136</v>
+      </c>
+      <c r="J71" s="16">
+        <f t="shared" si="5"/>
+        <v>27930</v>
+      </c>
+      <c r="K71" s="16">
+        <f t="shared" si="5"/>
+        <v>29136</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72">
-        <v>28900</v>
-      </c>
-      <c r="C72">
-        <v>28900</v>
-      </c>
-      <c r="D72">
-        <v>28900</v>
-      </c>
-      <c r="E72">
-        <v>28900</v>
-      </c>
-      <c r="F72">
-        <v>28900</v>
-      </c>
-      <c r="G72">
-        <v>28900</v>
-      </c>
-      <c r="H72">
-        <v>28900</v>
-      </c>
-      <c r="I72">
-        <v>28900</v>
-      </c>
-      <c r="J72">
-        <v>28900</v>
-      </c>
-      <c r="K72">
-        <v>28900</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>73</v>
-      </c>
-      <c r="G73">
-        <v>14000</v>
-      </c>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B74">
-        <v>3000</v>
+        <v>28900</v>
       </c>
       <c r="C74">
-        <v>3000</v>
+        <v>30900</v>
       </c>
       <c r="D74">
-        <v>3000</v>
+        <v>30900</v>
       </c>
       <c r="E74">
-        <v>3000</v>
+        <v>30900</v>
       </c>
       <c r="F74">
-        <v>3000</v>
+        <v>30900</v>
       </c>
       <c r="G74">
-        <v>3000</v>
+        <v>30900</v>
       </c>
       <c r="H74">
-        <v>3000</v>
+        <v>30900</v>
       </c>
       <c r="I74">
-        <v>3000</v>
+        <v>30900</v>
       </c>
       <c r="J74">
-        <v>3000</v>
+        <v>30900</v>
       </c>
       <c r="K74">
-        <v>3000</v>
+        <v>30900</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>73</v>
+      </c>
+      <c r="G75">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>71</v>
+      </c>
+      <c r="B76">
+        <v>3000</v>
+      </c>
+      <c r="C76">
+        <v>3000</v>
+      </c>
+      <c r="D76">
+        <v>3000</v>
+      </c>
+      <c r="E76">
+        <v>3000</v>
+      </c>
+      <c r="F76">
+        <v>3000</v>
+      </c>
+      <c r="G76">
+        <v>3000</v>
+      </c>
+      <c r="H76">
+        <v>3000</v>
+      </c>
+      <c r="I76">
+        <v>3000</v>
+      </c>
+      <c r="J76">
+        <v>3000</v>
+      </c>
+      <c r="K76">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
+    <row r="78" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B76" s="6">
-        <f t="shared" ref="B76:K76" si="5">SUM(B72:B75)</f>
+      <c r="B78" s="6">
+        <f t="shared" ref="B78:K78" si="6">SUM(B74:B77)</f>
         <v>31900</v>
       </c>
-      <c r="C76" s="6">
-        <f t="shared" si="5"/>
-        <v>31900</v>
-      </c>
-      <c r="D76" s="6">
-        <f t="shared" si="5"/>
-        <v>31900</v>
-      </c>
-      <c r="E76" s="6">
-        <f t="shared" si="5"/>
-        <v>31900</v>
-      </c>
-      <c r="F76" s="6">
-        <f t="shared" si="5"/>
-        <v>31900</v>
-      </c>
-      <c r="G76" s="6">
-        <f t="shared" si="5"/>
-        <v>45900</v>
-      </c>
-      <c r="H76" s="6">
-        <f t="shared" si="5"/>
-        <v>31900</v>
-      </c>
-      <c r="I76" s="6">
-        <f t="shared" si="5"/>
-        <v>31900</v>
-      </c>
-      <c r="J76" s="6">
-        <f t="shared" si="5"/>
-        <v>31900</v>
-      </c>
-      <c r="K76" s="6">
-        <f t="shared" si="5"/>
-        <v>31900</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+      <c r="C78" s="6">
+        <f t="shared" si="6"/>
+        <v>33900</v>
+      </c>
+      <c r="D78" s="6">
+        <f t="shared" si="6"/>
+        <v>33900</v>
+      </c>
+      <c r="E78" s="6">
+        <f t="shared" si="6"/>
+        <v>33900</v>
+      </c>
+      <c r="F78" s="6">
+        <f t="shared" si="6"/>
+        <v>33900</v>
+      </c>
+      <c r="G78" s="6">
+        <f t="shared" si="6"/>
+        <v>47900</v>
+      </c>
+      <c r="H78" s="6">
+        <f t="shared" si="6"/>
+        <v>33900</v>
+      </c>
+      <c r="I78" s="6">
+        <f t="shared" si="6"/>
+        <v>33900</v>
+      </c>
+      <c r="J78" s="6">
+        <f t="shared" si="6"/>
+        <v>33900</v>
+      </c>
+      <c r="K78" s="6">
+        <f t="shared" si="6"/>
+        <v>33900</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B78" s="2">
-        <f t="shared" ref="B78:K78" si="6">B76-B69</f>
+      <c r="B80" s="2">
+        <f t="shared" ref="B80:K80" si="7">B78-B71</f>
         <v>3473</v>
       </c>
-      <c r="C78" s="2">
-        <f t="shared" si="6"/>
-        <v>6794</v>
-      </c>
-      <c r="D78" s="2">
-        <f t="shared" si="6"/>
-        <v>3150</v>
-      </c>
-      <c r="E78" s="2">
-        <f t="shared" si="6"/>
-        <v>-2436</v>
-      </c>
-      <c r="F78" s="2">
-        <f t="shared" si="6"/>
-        <v>-307</v>
-      </c>
-      <c r="G78" s="2">
-        <f t="shared" si="6"/>
-        <v>12844</v>
-      </c>
-      <c r="H78" s="2">
-        <f t="shared" si="6"/>
-        <v>50</v>
-      </c>
-      <c r="I78" s="2">
-        <f t="shared" si="6"/>
-        <v>-1156</v>
-      </c>
-      <c r="J78" s="2">
-        <f t="shared" si="6"/>
-        <v>50</v>
-      </c>
-      <c r="K78" s="2">
-        <f t="shared" si="6"/>
-        <v>-1156</v>
+      <c r="C80" s="2">
+        <f t="shared" si="7"/>
+        <v>7264</v>
+      </c>
+      <c r="D80" s="2">
+        <f t="shared" si="7"/>
+        <v>4070</v>
+      </c>
+      <c r="E80" s="2">
+        <f t="shared" si="7"/>
+        <v>3484</v>
+      </c>
+      <c r="F80" s="2">
+        <f t="shared" si="7"/>
+        <v>5613</v>
+      </c>
+      <c r="G80" s="2">
+        <f t="shared" si="7"/>
+        <v>18764</v>
+      </c>
+      <c r="H80" s="2">
+        <f t="shared" si="7"/>
+        <v>5970</v>
+      </c>
+      <c r="I80" s="2">
+        <f t="shared" si="7"/>
+        <v>4764</v>
+      </c>
+      <c r="J80" s="2">
+        <f t="shared" si="7"/>
+        <v>5970</v>
+      </c>
+      <c r="K80" s="2">
+        <f t="shared" si="7"/>
+        <v>4764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>